<commit_message>
Set up autopush for Saurav
</commit_message>
<xml_diff>
--- a/speed-comparison-master/data/middleTRNew/MiddleTRNew.xlsx
+++ b/speed-comparison-master/data/middleTRNew/MiddleTRNew.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Student\ED-Assignment\speed-comparison-master\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/youyasushi/Desktop/UCT/Year 2/STA2005S/ED Project/speed-comparison-master/data/middleTRNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBCBFF1-2046-4D7B-95A3-7F4798227ED3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{138A1643-321F-5743-A099-C8638D9146B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22260" windowHeight="12640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
   <si>
     <t>C</t>
   </si>
@@ -106,9 +106,6 @@
     <t>383.4964066666666</t>
   </si>
   <si>
-    <t>473.79067999999995</t>
-  </si>
-  <si>
     <t>392.9250266666666</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
     <t>357.67083333333335</t>
   </si>
   <si>
-    <t>431.1397866666667</t>
-  </si>
-  <si>
     <t>434.40590000000003</t>
   </si>
   <si>
@@ -274,9 +268,6 @@
     <t>760.0442999999999</t>
   </si>
   <si>
-    <t>805.61044</t>
-  </si>
-  <si>
     <t>778.0431666666667</t>
   </si>
   <si>
@@ -376,9 +367,6 @@
     <t>3205.2069399999996</t>
   </si>
   <si>
-    <t>3495.404666666667</t>
-  </si>
-  <si>
     <t>74.4627199999995</t>
   </si>
   <si>
@@ -439,9 +427,6 @@
     <t>8046.358753333334</t>
   </si>
   <si>
-    <t>8647.631360000001</t>
-  </si>
-  <si>
     <t>8049.023019999999</t>
   </si>
   <si>
@@ -518,9 +503,6 @@
   </si>
   <si>
     <t>1858.8000133333335</t>
-  </si>
-  <si>
-    <t>1968.9265999999998</t>
   </si>
   <si>
     <t>1722.1296866666662</t>
@@ -599,7 +581,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -752,7 +734,7 @@
                   <c:v>1858.8000133333335</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1968.9265999999998</c:v>
+                  <c:v>1868.9266</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1795,12 +1777,12 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1820,558 +1802,558 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E8" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
-        <v>41</v>
+      <c r="B9">
+        <v>431.139786666666</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F9" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E10" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F10" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E11" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E12" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E14" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F14" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E15" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F16" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E17" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F17" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F18" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D19" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E19" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F19" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E20" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F20" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" t="s">
+        <v>132</v>
+      </c>
+      <c r="F21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>373.79067999999899</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22">
+        <v>765.61044000000004</v>
+      </c>
+      <c r="D22" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22">
+        <v>8047.6313600000003</v>
+      </c>
+      <c r="F22">
+        <v>1868.92659999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
         <v>53</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23">
+        <v>3195.40466666666</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" t="s">
+        <v>133</v>
+      </c>
+      <c r="F24" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" t="s">
+        <v>134</v>
+      </c>
+      <c r="F25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" t="s">
+        <v>135</v>
+      </c>
+      <c r="F26" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
         <v>81</v>
       </c>
-      <c r="D21" t="s">
-        <v>109</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="D27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E27" t="s">
         <v>136</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F27" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" t="s">
+        <v>111</v>
+      </c>
+      <c r="E28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F28" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" t="s">
-        <v>171</v>
-      </c>
-      <c r="E22" t="s">
-        <v>137</v>
-      </c>
-      <c r="F22" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" t="s">
+        <v>138</v>
+      </c>
+      <c r="F29" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" t="s">
-        <v>83</v>
-      </c>
-      <c r="D24" t="s">
-        <v>110</v>
-      </c>
-      <c r="E24" t="s">
-        <v>138</v>
-      </c>
-      <c r="F24" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" t="s">
-        <v>88</v>
-      </c>
-      <c r="D25" t="s">
-        <v>111</v>
-      </c>
-      <c r="E25" t="s">
-        <v>139</v>
-      </c>
-      <c r="F25" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" t="s">
-        <v>112</v>
-      </c>
-      <c r="E26" t="s">
-        <v>140</v>
-      </c>
-      <c r="F26" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27" t="s">
-        <v>113</v>
-      </c>
-      <c r="E27" t="s">
-        <v>141</v>
-      </c>
-      <c r="F27" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" t="s">
-        <v>114</v>
-      </c>
-      <c r="E28" t="s">
-        <v>142</v>
-      </c>
-      <c r="F28" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" t="s">
-        <v>115</v>
-      </c>
-      <c r="E29" t="s">
-        <v>143</v>
-      </c>
-      <c r="F29" t="s">
-        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>